<commit_message>
done pour 04-03: tomber + lingot or + pointage + niveau
</commit_message>
<xml_diff>
--- a/Planification Lode Runner.xlsx
+++ b/Planification Lode Runner.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.patel\Documents\Visual Studio Code WS\P46-Projet01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programmation 3D\Projet1\Lode Runner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECD22C66-65A2-44A1-ACF4-7C9671446B74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A61E7953-25E8-4A2F-9937-7B05B76A3CEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10665" yWindow="420" windowWidth="13440" windowHeight="13890" xr2:uid="{CF5DF6F3-6DC7-41D0-A2EB-7A2EBAE079CD}"/>
+    <workbookView xWindow="2100" yWindow="255" windowWidth="19140" windowHeight="15765" xr2:uid="{CF5DF6F3-6DC7-41D0-A2EB-7A2EBAE079CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -652,7 +654,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +809,7 @@
         <v>36</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>40</v>
@@ -817,17 +819,17 @@
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="20" t="s">
         <v>36</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -966,34 +968,34 @@
       <c r="A27" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="C27" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>37</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="C28" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>37</v>
       </c>
       <c r="E28" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="14" t="s">
-        <v>40</v>
+      <c r="F28" s="12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mouvement un peu meilleur
</commit_message>
<xml_diff>
--- a/Planification Lode Runner.xlsx
+++ b/Planification Lode Runner.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programmation 3D\Projet1\Lode Runner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1648C5F1-4629-4C67-AF7D-3EF8A4649537}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66304BF2-FA3B-419A-82CA-41DBB810EA09}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10665" yWindow="420" windowWidth="13440" windowHeight="13890" xr2:uid="{CF5DF6F3-6DC7-41D0-A2EB-7A2EBAE079CD}"/>
   </bookViews>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="47">
   <si>
     <t>Décor</t>
   </si>
@@ -168,6 +166,12 @@
   </si>
   <si>
     <t>Complété tôt</t>
+  </si>
+  <si>
+    <t>Complété tard</t>
+  </si>
+  <si>
+    <t>Complété à temps</t>
   </si>
 </sst>
 </file>
@@ -248,7 +252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -285,6 +289,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -307,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -337,6 +353,8 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -653,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17FB730C-8DFC-4F8E-B8DC-E7BD908766F6}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,10 +723,10 @@
       <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="22" t="s">
         <v>22</v>
       </c>
       <c r="E6" t="s">
@@ -763,6 +781,9 @@
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
+      <c r="H11" s="21" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -780,6 +801,9 @@
       <c r="F12" s="12" t="s">
         <v>24</v>
       </c>
+      <c r="H12" s="22" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
@@ -802,10 +826,10 @@
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E14" t="s">
@@ -836,10 +860,10 @@
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E16" t="s">
@@ -853,10 +877,10 @@
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="22" t="s">
         <v>36</v>
       </c>
       <c r="E17" t="s">
@@ -875,10 +899,10 @@
       <c r="A20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E20" t="s">
@@ -892,10 +916,10 @@
       <c r="A21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E21" t="s">
@@ -909,27 +933,27 @@
       <c r="A22" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E22" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="14" t="s">
-        <v>40</v>
+      <c r="F22" s="12" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E23" t="s">
@@ -943,10 +967,10 @@
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="21" t="s">
         <v>36</v>
       </c>
       <c r="E24" t="s">

</xml_diff>